<commit_message>
no change in code
</commit_message>
<xml_diff>
--- a/InventoryManagement.Console.API/DB/InventoryDB.xlsx
+++ b/InventoryManagement.Console.API/DB/InventoryDB.xlsx
@@ -2532,7 +2532,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2587,7 +2587,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>23456</v>
+        <v>123456</v>
       </c>
       <c r="E3">
         <v>11111</v>

</xml_diff>